<commit_message>
Add use_label to flextable() and use glue_data(.x = .SD) to summarise
</commit_message>
<xml_diff>
--- a/output/checks/dft2_table_for_sending_individual_reports.xlsx
+++ b/output/checks/dft2_table_for_sending_individual_reports.xlsx
@@ -385,7 +385,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_10_2024-02-05.docx</t>
+          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_10_2024-12-02.docx</t>
         </is>
       </c>
     </row>
@@ -400,7 +400,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_11_2024-02-05.docx</t>
+          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_11_2024-12-02.docx</t>
         </is>
       </c>
     </row>
@@ -415,7 +415,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_13_2024-02-05.docx</t>
+          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_13_2024-12-02.docx</t>
         </is>
       </c>
     </row>
@@ -430,7 +430,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_15_2024-02-05.docx</t>
+          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_15_2024-12-02.docx</t>
         </is>
       </c>
     </row>
@@ -445,7 +445,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_16_2024-02-05.docx</t>
+          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_16_2024-12-02.docx</t>
         </is>
       </c>
     </row>
@@ -460,7 +460,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_17_2024-02-05.docx</t>
+          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_17_2024-12-02.docx</t>
         </is>
       </c>
     </row>
@@ -475,7 +475,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_18_2024-02-05.docx</t>
+          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_18_2024-12-02.docx</t>
         </is>
       </c>
     </row>
@@ -490,7 +490,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_19_2024-02-05.docx</t>
+          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_19_2024-12-02.docx</t>
         </is>
       </c>
     </row>
@@ -505,7 +505,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_20_2024-02-05.docx</t>
+          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_20_2024-12-02.docx</t>
         </is>
       </c>
     </row>
@@ -520,7 +520,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_21_2024-02-05.docx</t>
+          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_21_2024-12-02.docx</t>
         </is>
       </c>
     </row>
@@ -535,7 +535,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_22_2024-02-05.docx</t>
+          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_22_2024-12-02.docx</t>
         </is>
       </c>
     </row>
@@ -550,7 +550,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_23_2024-02-05.docx</t>
+          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_23_2024-12-02.docx</t>
         </is>
       </c>
     </row>
@@ -565,7 +565,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_24_2024-02-05.docx</t>
+          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_24_2024-12-02.docx</t>
         </is>
       </c>
     </row>
@@ -580,7 +580,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_25_2024-02-05.docx</t>
+          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_25_2024-12-02.docx</t>
         </is>
       </c>
     </row>
@@ -595,7 +595,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_26_2024-02-05.docx</t>
+          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_26_2024-12-02.docx</t>
         </is>
       </c>
     </row>
@@ -610,7 +610,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_2_2024-02-05.docx</t>
+          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_2_2024-12-02.docx</t>
         </is>
       </c>
     </row>
@@ -625,7 +625,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_3_2024-02-05.docx</t>
+          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_3_2024-12-02.docx</t>
         </is>
       </c>
     </row>
@@ -640,7 +640,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_4_2024-02-05.docx</t>
+          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_4_2024-12-02.docx</t>
         </is>
       </c>
     </row>
@@ -655,7 +655,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_5_2024-02-05.docx</t>
+          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_5_2024-12-02.docx</t>
         </is>
       </c>
     </row>
@@ -670,7 +670,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_6_2024-02-05.docx</t>
+          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_6_2024-12-02.docx</t>
         </is>
       </c>
     </row>
@@ -685,7 +685,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_7_2024-02-05.docx</t>
+          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_7_2024-12-02.docx</t>
         </is>
       </c>
     </row>
@@ -700,7 +700,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_8_2024-02-05.docx</t>
+          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_8_2024-12-02.docx</t>
         </is>
       </c>
     </row>
@@ -715,7 +715,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_9_2024-02-05.docx</t>
+          <t>C:/Users/ol8094/Documents/_analyses/_delphi_ft_various/delphi-fast-track-demo/output/reports/dft2/report_by_participant/dft2_report_participant_9_2024-12-02.docx</t>
         </is>
       </c>
     </row>

</xml_diff>